<commit_message>
Modifing S_PM_05.xlsx File to S_PM_05 Folder on PM_CC Folder
</commit_message>
<xml_diff>
--- a/PM_CC/S_PM_05/S_PM_05.xlsx
+++ b/PM_CC/S_PM_05/S_PM_05.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Developing&amp;Training_Cost" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,10 +160,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -448,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:K8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,33 +467,33 @@
     <row r="1" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
@@ -525,10 +528,10 @@
         <v>3</v>
       </c>
       <c r="J6" s="1">
-        <v>40</v>
-      </c>
-      <c r="K6" s="4">
-        <v>2400</v>
+        <v>480</v>
+      </c>
+      <c r="K6" s="12">
+        <v>28800</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -540,10 +543,10 @@
         <v>4</v>
       </c>
       <c r="J7" s="1">
-        <v>20</v>
-      </c>
-      <c r="K7" s="4">
-        <v>1000</v>
+        <v>160</v>
+      </c>
+      <c r="K7" s="12">
+        <v>8000</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -555,10 +558,10 @@
         <v>7</v>
       </c>
       <c r="J8" s="1">
-        <v>10</v>
-      </c>
-      <c r="K8" s="4">
-        <v>400</v>
+        <v>80</v>
+      </c>
+      <c r="K8" s="12">
+        <v>3200</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -597,7 +600,7 @@
   <dimension ref="A6:K12"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,8 +625,8 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4">
-        <v>5000</v>
+      <c r="B7" s="12">
+        <v>10000</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -664,7 +667,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,8 +683,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>8800</v>
+      <c r="A2" s="12">
+        <v>50000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -702,7 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -713,7 +716,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>